<commit_message>
changed from tkinter to win32clipboard
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Çizelge2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Çizelge3" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -17,6 +17,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">peinlich</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -119,81 +127,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>